<commit_message>
csv files added for db. Queries worked on
</commit_message>
<xml_diff>
--- a/course project/data files/suppliers.xlsx
+++ b/course project/data files/suppliers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ENSF607\ENSF-607-608-Term-Project\course project\data files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDE00E2-F682-46D0-B580-1547C449E5C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F35DCEF-0245-4D55-A2F9-999511B8D871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="2220" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4545" yWindow="2880" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet3!$A$1:$D$21</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet3!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,19 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Grommet Builders</t>
   </si>
@@ -233,16 +221,28 @@
   </si>
   <si>
     <t>Wing</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>Local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,17 +275,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -296,32 +286,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{959E68FD-9F71-4BBA-B2C1-9B5F7CD8953E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
-      <queryTableField id="1" name="Column1" tableColumnId="1"/>
-      <queryTableField id="2" name="Column2" tableColumnId="2"/>
-      <queryTableField id="3" name="Column3" tableColumnId="3"/>
-      <queryTableField id="4" name="Column4" tableColumnId="4"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{30D0D08E-7A4F-47FD-B3B9-CA4790F98A31}" name="suppliers_old__2" displayName="suppliers_old__2" ref="A1:D21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D21" xr:uid="{1D3256F0-4E32-445B-A5F6-8B9613EF91B4}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{25F122BF-AE0A-493A-899F-B6020133380B}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{0DF7CA5D-6A26-4045-8FBA-CD8CCD9AA207}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{86F33244-A2D2-4998-B10A-469956495A49}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{D6C8892A-8EDD-4B79-AE30-E6B349261EA7}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,317 +551,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10521C52-BABF-43C7-8AD5-E79783F81881}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>8001</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8002</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8001</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8003</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>8002</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8004</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8003</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8005</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8004</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8006</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8005</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8007</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>8006</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8008</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8007</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8009</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8008</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8010</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8009</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8011</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8010</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8012</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8011</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8013</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8012</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8014</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8013</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8015</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>8014</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8016</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8015</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8017</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>8016</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8018</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>8017</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8019</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8018</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8020</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>8019</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>8020</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>63</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>